<commit_message>
Last update with straffen
</commit_message>
<xml_diff>
--- a/#Persönliche Dokument/Reunion Liste avec Inscription.xlsx
+++ b/#Persönliche Dokument/Reunion Liste avec Inscription.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilno\Desktop\#Persönliche Dokument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilno\Desktop\Git@Dokument\Dokument\#Persönliche Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667BCCAC-4BBF-4CF4-BCBF-67AEFE91F82A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D0DF3E-2AB8-4F56-A02F-09CF507C479D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,8 +41,10 @@
     <author>brice onla</author>
     <author>tc={DD0F6CE0-1017-4556-A11A-298CC5D3F45C}</author>
     <author>tc={691BF698-0B81-43AA-83A4-964E649476A3}</author>
+    <author>tc={A0819D31-0965-469D-B7F3-737C6F1771A5}</author>
     <author>tc={187BC417-5EF6-423D-96E9-F943947C2E91}</author>
     <author>tc={FEB8E99A-E773-4B78-B218-1345E1F8D7A2}</author>
+    <author>tc={83EF4D72-BE90-43D4-BA70-57B790059924}</author>
     <author>tc={280FF80F-97CE-4945-AFCB-019F269A4081}</author>
     <author>tc={41C82386-30BC-4A70-B77E-C6F60BF2632D}</author>
     <author>tc={E749B736-D25B-4AA8-A2F9-E69703856A28}</author>
@@ -218,7 +222,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="N7" authorId="3" shapeId="0" xr:uid="{187BC417-5EF6-423D-96E9-F943947C2E91}">
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{21AF5716-CFBA-4797-B5E9-D285A9867B26}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>brice onla:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Beweis nachgereicht 
+geht oder nicht ?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="3" shapeId="0" xr:uid="{A0819D31-0965-469D-B7F3-737C6F1771A5}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    argent des 2 dernier mois</t>
+      </text>
+    </comment>
+    <comment ref="N7" authorId="4" shapeId="0" xr:uid="{187BC417-5EF6-423D-96E9-F943947C2E91}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -226,7 +263,7 @@
     Il na pas payer son Straffen</t>
       </text>
     </comment>
-    <comment ref="O7" authorId="4" shapeId="0" xr:uid="{FEB8E99A-E773-4B78-B218-1345E1F8D7A2}">
+    <comment ref="O7" authorId="5" shapeId="0" xr:uid="{FEB8E99A-E773-4B78-B218-1345E1F8D7A2}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -234,7 +271,15 @@
     Il na pas payer son Straffen</t>
       </text>
     </comment>
-    <comment ref="J8" authorId="5" shapeId="0" xr:uid="{280FF80F-97CE-4945-AFCB-019F269A4081}">
+    <comment ref="P7" authorId="6" shapeId="0" xr:uid="{83EF4D72-BE90-43D4-BA70-57B790059924}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Il na pas payer son Straffen</t>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="7" shapeId="0" xr:uid="{280FF80F-97CE-4945-AFCB-019F269A4081}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -242,7 +287,7 @@
     Jael a payer sa chez lui</t>
       </text>
     </comment>
-    <comment ref="L10" authorId="6" shapeId="0" xr:uid="{41C82386-30BC-4A70-B77E-C6F60BF2632D}">
+    <comment ref="L10" authorId="8" shapeId="0" xr:uid="{41C82386-30BC-4A70-B77E-C6F60BF2632D}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -250,7 +295,7 @@
     Joel a remis une Somme de 10€</t>
       </text>
     </comment>
-    <comment ref="L12" authorId="7" shapeId="0" xr:uid="{E749B736-D25B-4AA8-A2F9-E69703856A28}">
+    <comment ref="L12" authorId="9" shapeId="0" xr:uid="{E749B736-D25B-4AA8-A2F9-E69703856A28}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -258,7 +303,7 @@
     Valona a paye sa etant facher</t>
       </text>
     </comment>
-    <comment ref="M13" authorId="8" shapeId="0" xr:uid="{8020C977-8E31-4C9E-B618-9329B8C2E673}">
+    <comment ref="M13" authorId="10" shapeId="0" xr:uid="{8020C977-8E31-4C9E-B618-9329B8C2E673}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -266,7 +311,7 @@
     Il a payer sofort</t>
       </text>
     </comment>
-    <comment ref="N14" authorId="9" shapeId="0" xr:uid="{92186A68-CEEE-4922-A858-72C439FC0FB2}">
+    <comment ref="N14" authorId="11" shapeId="0" xr:uid="{92186A68-CEEE-4922-A858-72C439FC0FB2}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -304,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t xml:space="preserve">La Reunion </t>
   </si>
@@ -448,13 +493,16 @@
   </si>
   <si>
     <t>Status Amande Juin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233 dans la case </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <name val="Tw Cen MT Condensed"/>
@@ -516,6 +564,19 @@
       <name val="Adobe Caslon Pro"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tw Cen MT Condensed"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -569,7 +630,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -612,13 +673,23 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Nummer" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -972,9 +1043,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Hochzeits-Gästeliste" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Hochzeits-Gästeliste" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1190,24 +1261,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Gästeliste" displayName="Gästeliste" ref="C2:N17" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Gästeliste" displayName="Gästeliste" ref="C2:N17" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="C2:N17" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nom"/>
-    <tableColumn id="4" xr3:uid="{0B0CDBAF-04A5-44C9-97E9-4B4134B80C4A}" name="Prenom" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{0B0CDBAF-04A5-44C9-97E9-4B4134B80C4A}" name="Prenom" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="function du membre "/>
-    <tableColumn id="5" xr3:uid="{CAF249CA-F733-4C2B-B962-F0B05A70831A}" name="Inscription apercus " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{AD98409C-CB0B-4083-8B5D-22B36D614007}" name=" Case " dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{3F72D1D8-379E-443E-AF53-41B05461B167}" name="Amande avant 19 Jan" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{59F18DB4-819A-4500-ACFB-330111725D1F}" name="Amande du 19 jan" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{699FA6FE-2223-4D8B-929A-8A91EB14723B}" name="Amande de Feb" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{387C15B6-C9F8-42AE-92DE-F7559155889E}" name="Status Amande Mars" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{D464E616-47D3-419D-8AAB-D30858DB8718}" name="Status Amande Avril" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{D0B7D434-6763-444E-9409-16524B3B9CB6}" name="Status Amande 22" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{8F7917C0-84DD-4754-8F8E-04D05D36D7FD}" name="Status Amande Juin" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{CAF249CA-F733-4C2B-B962-F0B05A70831A}" name="Inscription apercus " dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{AD98409C-CB0B-4083-8B5D-22B36D614007}" name=" Case " dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3F72D1D8-379E-443E-AF53-41B05461B167}" name="Amande avant 19 Jan" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{59F18DB4-819A-4500-ACFB-330111725D1F}" name="Amande du 19 jan" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{699FA6FE-2223-4D8B-929A-8A91EB14723B}" name="Amande de Feb" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{387C15B6-C9F8-42AE-92DE-F7559155889E}" name="Status Amande Mars" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{D464E616-47D3-419D-8AAB-D30858DB8718}" name="Status Amande Avril" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{D0B7D434-6763-444E-9409-16524B3B9CB6}" name="Status Amande 22" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{8F7917C0-84DD-4754-8F8E-04D05D36D7FD}" name="Status Amande Juin" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Hochzeits-Gästeliste" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1451,10 +1522,16 @@
   <threadedComment ref="J4" dT="2019-05-29T13:26:39.28" personId="{8E14C7C1-4E9D-4D2B-BD7D-8154D1C490EA}" id="{691BF698-0B81-43AA-83A4-964E649476A3}">
     <text>Il a donner ke 2€</text>
   </threadedComment>
+  <threadedComment ref="G7" dT="2019-10-20T14:18:06.28" personId="{8E14C7C1-4E9D-4D2B-BD7D-8154D1C490EA}" id="{A0819D31-0965-469D-B7F3-737C6F1771A5}">
+    <text>argent des 2 dernier mois</text>
+  </threadedComment>
   <threadedComment ref="N7" dT="2019-05-29T13:27:41.80" personId="{8E14C7C1-4E9D-4D2B-BD7D-8154D1C490EA}" id="{187BC417-5EF6-423D-96E9-F943947C2E91}">
     <text>Il na pas payer son Straffen</text>
   </threadedComment>
   <threadedComment ref="O7" dT="2019-05-29T13:27:41.80" personId="{8E14C7C1-4E9D-4D2B-BD7D-8154D1C490EA}" id="{FEB8E99A-E773-4B78-B218-1345E1F8D7A2}">
+    <text>Il na pas payer son Straffen</text>
+  </threadedComment>
+  <threadedComment ref="P7" dT="2019-05-29T13:27:41.80" personId="{8E14C7C1-4E9D-4D2B-BD7D-8154D1C490EA}" id="{83EF4D72-BE90-43D4-BA70-57B790059924}">
     <text>Il na pas payer son Straffen</text>
   </threadedComment>
   <threadedComment ref="J8" dT="2019-05-29T13:30:34.81" personId="{8E14C7C1-4E9D-4D2B-BD7D-8154D1C490EA}" id="{280FF80F-97CE-4945-AFCB-019F269A4081}">
@@ -1481,13 +1558,13 @@
     <tabColor theme="8"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6328125" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
@@ -1504,14 +1581,18 @@
     <col min="13" max="13" width="20.453125" customWidth="1"/>
     <col min="14" max="14" width="27.453125" customWidth="1"/>
     <col min="15" max="15" width="27.453125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="75" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:16" ht="75" customHeight="1">
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="O1" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="2" spans="2:16" ht="30" customHeight="1">
       <c r="B2" s="8"/>
       <c r="C2" s="10" t="s">
         <v>2</v>
@@ -1552,8 +1633,11 @@
       <c r="O2" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="P2" s="10" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="3" spans="2:16" ht="30" customHeight="1">
       <c r="B3" s="8">
         <v>1</v>
       </c>
@@ -1596,8 +1680,11 @@
       <c r="O3" s="9">
         <v>0</v>
       </c>
+      <c r="P3" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="4" spans="2:16" ht="30" customHeight="1">
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -1640,8 +1727,11 @@
       <c r="O4" s="9">
         <v>0</v>
       </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="5" spans="2:16" ht="30" customHeight="1">
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -1684,8 +1774,11 @@
       <c r="O5" s="9">
         <v>-5</v>
       </c>
+      <c r="P5" s="9">
+        <v>-5</v>
+      </c>
     </row>
-    <row r="6" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="6" spans="2:16" ht="30" customHeight="1">
       <c r="B6" s="8">
         <v>4</v>
       </c>
@@ -1728,8 +1821,11 @@
       <c r="O6" s="9">
         <v>0</v>
       </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="7" spans="2:16" ht="30" customHeight="1">
       <c r="B7" s="8">
         <v>5</v>
       </c>
@@ -1746,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H7" s="12">
         <v>2</v>
@@ -1772,8 +1868,11 @@
       <c r="O7" s="11">
         <v>-7</v>
       </c>
+      <c r="P7" s="11">
+        <v>-7</v>
+      </c>
     </row>
-    <row r="8" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="8" spans="2:16" ht="30" customHeight="1">
       <c r="B8" s="8">
         <v>6</v>
       </c>
@@ -1816,8 +1915,11 @@
       <c r="O8" s="11">
         <v>-5</v>
       </c>
+      <c r="P8" s="11">
+        <v>-5</v>
+      </c>
     </row>
-    <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="9" spans="2:16" ht="30" customHeight="1">
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -1860,8 +1962,11 @@
       <c r="O9" s="11">
         <v>0</v>
       </c>
+      <c r="P9" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="10" spans="2:16" ht="30" customHeight="1">
       <c r="B10" s="8">
         <v>8</v>
       </c>
@@ -1904,8 +2009,11 @@
       <c r="O10" s="11">
         <v>0</v>
       </c>
+      <c r="P10" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="11" spans="2:16" ht="30" customHeight="1">
       <c r="B11" s="8">
         <v>9</v>
       </c>
@@ -1948,8 +2056,11 @@
       <c r="O11" s="11">
         <v>0</v>
       </c>
+      <c r="P11" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="12" spans="2:16" ht="30" customHeight="1">
       <c r="B12" s="8">
         <v>10</v>
       </c>
@@ -1992,8 +2103,11 @@
       <c r="O12" s="11">
         <v>0</v>
       </c>
+      <c r="P12" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="13" spans="2:16" ht="30" customHeight="1">
       <c r="B13" s="8">
         <v>11</v>
       </c>
@@ -2036,8 +2150,11 @@
       <c r="O13" s="11">
         <v>0</v>
       </c>
+      <c r="P13" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="14" spans="2:16" ht="30" customHeight="1">
       <c r="B14" s="8">
         <v>12</v>
       </c>
@@ -2080,8 +2197,11 @@
       <c r="O14" s="11">
         <v>0</v>
       </c>
+      <c r="P14" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="2:15" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="15" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B15" s="8">
         <v>13</v>
       </c>
@@ -2124,8 +2244,11 @@
       <c r="O15" s="11">
         <v>0</v>
       </c>
+      <c r="P15" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="2:15" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="16" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="11"/>
@@ -2136,7 +2259,7 @@
       </c>
       <c r="G16" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H16" s="11">
         <f t="shared" si="0"/>
@@ -2168,8 +2291,11 @@
       <c r="O16" s="11">
         <v>0</v>
       </c>
+      <c r="P16" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:15" ht="30" customHeight="1">
       <c r="C17" s="4" t="s">
         <v>46</v>
       </c>
@@ -2182,7 +2308,7 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F16,G16,H16,J17)</f>
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="G17"/>
       <c r="H17" s="2"/>
@@ -2197,12 +2323,60 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="19" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="3:15" ht="30" customHeight="1">
       <c r="C19" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F3:F17">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F16">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G15">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G15">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H15">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -2214,7 +2388,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F16">
+  <conditionalFormatting sqref="H3:H15">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -2226,7 +2400,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G15">
+  <conditionalFormatting sqref="I3:I15">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -2238,7 +2412,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G15">
+  <conditionalFormatting sqref="I3:I15">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -2250,7 +2424,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H15">
+  <conditionalFormatting sqref="G16">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -2262,7 +2436,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H15">
+  <conditionalFormatting sqref="H16">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -2274,7 +2448,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -2286,7 +2460,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I15">
+  <conditionalFormatting sqref="F3:F15">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -2298,19 +2472,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
+  <conditionalFormatting sqref="J3:J15">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2322,7 +2484,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="J3:J15">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2334,7 +2496,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F15">
+  <conditionalFormatting sqref="J16">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2346,7 +2508,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J15">
+  <conditionalFormatting sqref="K3:K15">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2358,7 +2520,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J15">
+  <conditionalFormatting sqref="K3:K15">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2370,7 +2532,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
+  <conditionalFormatting sqref="K16">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2382,7 +2544,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K15">
+  <conditionalFormatting sqref="L3:L15">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2394,7 +2556,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K15">
+  <conditionalFormatting sqref="L3:L15">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2406,7 +2568,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="L16">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2418,7 +2580,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L15">
+  <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2430,7 +2592,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L15">
+  <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2442,7 +2604,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16">
+  <conditionalFormatting sqref="M16">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2454,7 +2616,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M15">
+  <conditionalFormatting sqref="N3:N15">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2466,7 +2628,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M15">
+  <conditionalFormatting sqref="N3:N15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2478,7 +2640,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
+  <conditionalFormatting sqref="N16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2490,7 +2652,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N15">
+  <conditionalFormatting sqref="O3:O15">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2502,7 +2664,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N15">
+  <conditionalFormatting sqref="O3:O15">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2514,7 +2676,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="O16">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2526,7 +2688,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O15">
+  <conditionalFormatting sqref="P3:P15">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2538,7 +2700,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O15">
+  <conditionalFormatting sqref="P3:P15">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2550,7 +2712,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O16">
+  <conditionalFormatting sqref="P16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2565,7 +2727,7 @@
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift den Namen des Gastes ein." sqref="C2:D2" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Erstellen Sie auf diesem Arbeitsblatt mit einer Hochzeits-Gästeliste eine Liste der Gäste." sqref="A1:G1" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift Stadt und Postleitzahl ein." sqref="E2:O2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift Stadt und Postleitzahl ein." sqref="E2:P2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2582,7 +2744,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{A8F29EF6-AC24-44E0-8BAE-E933DBF79B23}">
+          <x14:cfRule type="containsText" priority="29" operator="containsText" id="{A8F29EF6-AC24-44E0-8BAE-E933DBF79B23}">
             <xm:f>NOT(ISERROR(SEARCH("-",D3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2596,7 +2758,7 @@
           <xm:sqref>D3:I17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{6108245F-F08A-4092-9BC3-9695375896FD}">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{6108245F-F08A-4092-9BC3-9695375896FD}">
             <xm:f>NOT(ISERROR(SEARCH("-",J3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2610,7 +2772,7 @@
           <xm:sqref>J3:J16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{D693FAAE-3A33-4C3B-AED7-85A962BBB003}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{D693FAAE-3A33-4C3B-AED7-85A962BBB003}">
             <xm:f>NOT(ISERROR(SEARCH("-",K3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2624,7 +2786,7 @@
           <xm:sqref>K3:K16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{CE9B2254-16FB-4FEF-A249-F2CCB50FE2F5}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{CE9B2254-16FB-4FEF-A249-F2CCB50FE2F5}">
             <xm:f>NOT(ISERROR(SEARCH("-",L3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2638,7 +2800,7 @@
           <xm:sqref>L3:L16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{EEFE299F-DC81-4200-8EE0-014664809B59}">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{EEFE299F-DC81-4200-8EE0-014664809B59}">
             <xm:f>NOT(ISERROR(SEARCH("-",M3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2652,7 +2814,7 @@
           <xm:sqref>M3:M16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{0AF1F4F5-5A33-4FAD-93F0-0393D1CA3796}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{0AF1F4F5-5A33-4FAD-93F0-0393D1CA3796}">
             <xm:f>NOT(ISERROR(SEARCH("-",N3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2666,7 +2828,7 @@
           <xm:sqref>N3:N16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{8C6DE634-0DD7-45CF-9590-D18CFB970514}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{8C6DE634-0DD7-45CF-9590-D18CFB970514}">
             <xm:f>NOT(ISERROR(SEARCH("-",O3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2679,6 +2841,20 @@
           </x14:cfRule>
           <xm:sqref>O3:O16</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{3EDAEF2B-2B43-4D32-8B8F-75875F63DF45}">
+            <xm:f>NOT(ISERROR(SEARCH("-",P3)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>P3:P16</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>